<commit_message>
Basic data for class 4 added
</commit_message>
<xml_diff>
--- a/DA exl Classass.xlsx
+++ b/DA exl Classass.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Digital Analysis YT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA Analytics Study data\Digital Analysis 3.0M\Excel-YT-Classes-Data\Excel-Classes-Excel-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14830BBF-2CCB-4514-8B76-D501E9A25403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0724250-281E-46AA-BC5D-7AD921852C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{F6D9AFDF-A79F-445E-826E-10108AB2203E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F6D9AFDF-A79F-445E-826E-10108AB2203E}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>MS Excel</t>
   </si>
@@ -177,13 +175,16 @@
   </si>
   <si>
     <t>Zoom  Navigation </t>
+  </si>
+  <si>
+    <t>Main Topics To Be Discussed in MS Excel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,15 +203,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -235,19 +227,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -539,85 +534,85 @@
   <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -956,425 +951,429 @@
   <dimension ref="B1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.85546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="3" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.875" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.625" customWidth="1"/>
+    <col min="4" max="4" width="13.875" customWidth="1"/>
+    <col min="5" max="5" width="4.75" customWidth="1"/>
+    <col min="6" max="6" width="3" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="61.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+    <row r="1" spans="2:13">
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="2:13">
+      <c r="B2" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="E2" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="19" t="s">
+      <c r="M2" s="36"/>
+    </row>
+    <row r="3" spans="2:13">
+      <c r="B3" s="40"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="42"/>
+      <c r="F3" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="35"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="24"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+    </row>
+    <row r="4" spans="2:13">
+      <c r="B4" s="7"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="8"/>
+      <c r="F4" s="25">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="24"/>
+    </row>
+    <row r="5" spans="2:13" ht="15">
+      <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="10"/>
+      <c r="F5" s="25">
+        <v>2</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="24"/>
+      <c r="L5" s="30">
         <v>1</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="M5" s="32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="15">
+      <c r="B6" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="12"/>
+      <c r="F6" s="25">
+        <v>3</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="24"/>
+      <c r="L6" s="30">
         <v>2</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="M6" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="15">
+      <c r="B7" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="10"/>
+      <c r="F7" s="25">
+        <v>4</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="24"/>
+      <c r="L7" s="30">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="24"/>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E4" s="7"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="8"/>
-      <c r="I4" s="25">
-        <v>1</v>
-      </c>
-      <c r="J4" s="6" t="s">
+      <c r="M7" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="15">
+      <c r="B8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="12"/>
+      <c r="F8" s="25">
+        <v>5</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="24"/>
+      <c r="L8" s="30">
         <v>4</v>
       </c>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="24"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="39">
-        <v>1</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="10"/>
-      <c r="I5" s="25">
-        <v>2</v>
-      </c>
-      <c r="J5" s="6" t="s">
+      <c r="M8" s="32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13">
+      <c r="B9" s="14"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="10"/>
+      <c r="F9" s="25">
+        <v>6</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="24"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13">
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="F10" s="25">
+        <v>7</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="24"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="15">
+      <c r="F11" s="25">
+        <v>8</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="24"/>
+      <c r="L11" s="30">
         <v>5</v>
       </c>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="24"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="39">
-        <v>2</v>
-      </c>
-      <c r="C6" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="12"/>
-      <c r="I6" s="25">
-        <v>3</v>
-      </c>
-      <c r="J6" s="6" t="s">
+      <c r="M11" s="33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13">
+      <c r="F12" s="25">
+        <v>9</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="24"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13">
+      <c r="F13" s="25">
+        <v>10</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="24"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13">
+      <c r="F14" s="25">
+        <v>11</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="24"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13">
+      <c r="F15" s="25">
+        <v>12</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="24"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="15">
+      <c r="F16" s="25">
+        <v>13</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="24"/>
+      <c r="L16" s="30">
         <v>6</v>
       </c>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="24"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="39">
-        <v>3</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="10"/>
-      <c r="I7" s="25">
-        <v>4</v>
-      </c>
-      <c r="J7" s="6" t="s">
+      <c r="M16" s="32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="6:13">
+      <c r="F17" s="25">
+        <v>14</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="24"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="6:13">
+      <c r="F18" s="25">
+        <v>15</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="24"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="6:13">
+      <c r="F19" s="25">
+        <v>16</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="24"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="6:13">
+      <c r="F20" s="25">
+        <v>17</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="24"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="6:13">
+      <c r="F21" s="25">
+        <v>18</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="24"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="6:13">
+      <c r="F22" s="25">
+        <v>19</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="24"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="6:13" ht="15">
+      <c r="F23" s="26">
+        <v>20</v>
+      </c>
+      <c r="G23" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="29"/>
+      <c r="L23" s="30">
         <v>7</v>
       </c>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="24"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="39">
-        <v>4</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="12"/>
-      <c r="I8" s="25">
-        <v>5</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="24"/>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="39"/>
-      <c r="C9" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="10"/>
-      <c r="I9" s="25">
-        <v>6</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="24"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="39"/>
-      <c r="C10" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
-      <c r="I10" s="25">
-        <v>7</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="24"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="39">
-        <v>5</v>
-      </c>
-      <c r="C11" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="25">
-        <v>8</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="24"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="39"/>
-      <c r="C12" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12" s="25">
-        <v>9</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="24"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="39"/>
-      <c r="C13" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="I13" s="25">
-        <v>10</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="24"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="39"/>
-      <c r="C14" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="25">
-        <v>11</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="24"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="39"/>
-      <c r="C15" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="I15" s="25">
-        <v>12</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="24"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="39">
-        <v>6</v>
-      </c>
-      <c r="C16" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="I16" s="25">
-        <v>13</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="24"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="39"/>
-      <c r="C17" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" s="25">
-        <v>14</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="24"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="39"/>
-      <c r="C18" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="I18" s="25">
-        <v>15</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="24"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="39"/>
-      <c r="C19" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="I19" s="25">
-        <v>16</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="24"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="39"/>
-      <c r="C20" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="I20" s="25">
-        <v>17</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="24"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="39"/>
-      <c r="C21" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="I21" s="25">
-        <v>18</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="24"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="39"/>
-      <c r="C22" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="I22" s="25">
-        <v>19</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="24"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="39">
-        <v>7</v>
-      </c>
-      <c r="C23" s="41" t="s">
+      <c r="M23" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="I23" s="26">
-        <v>20</v>
-      </c>
-      <c r="J23" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="29"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="39"/>
-      <c r="C24" s="40" t="s">
+    </row>
+    <row r="24" spans="6:13">
+      <c r="L24" s="30"/>
+      <c r="M24" s="31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="39"/>
-      <c r="C25" s="40" t="s">
+    <row r="25" spans="6:13">
+      <c r="L25" s="30"/>
+      <c r="M25" s="31" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="39"/>
-      <c r="C26" s="40" t="s">
+    <row r="26" spans="6:13">
+      <c r="L26" s="30"/>
+      <c r="M26" s="31" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="E2:G3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="L2:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>